<commit_message>
using numericInput for VOC
</commit_message>
<xml_diff>
--- a/Template_CoMoCOVID-19App_v19.xlsx
+++ b/Template_CoMoCOVID-19App_v19.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivier/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivier/Documents/Projets/CoMo/como/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C298E3A-5E61-ED47-9FF1-C54B4B44E54C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C6A32B8-0E36-F747-95E1-990326F41754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25820" windowHeight="14160" tabRatio="648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="501">
   <si>
     <t>Template v19</t>
   </si>
@@ -3223,7 +3223,7 @@
     <t>To fill out the 'Value' in the VOC sheet you need to know what the frequency of each variant is, and what effect on the relevant parameter that variant has. For example, alpha variant has 20% increased transmissibility and delta variant has 60% increased transmissibility. If at time t you have 20% Sars-CoV-2, 30% alpha and 50% delta, you can calculate RR for transmissibility as (see the formula below):</t>
   </si>
   <si>
-    <t>v19.d</t>
+    <t>v19.e</t>
   </si>
 </sst>
 </file>
@@ -4166,7 +4166,7 @@
   <dimension ref="A1:F76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -4552,7 +4552,7 @@
   <dimension ref="A1:G100"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -4600,7 +4600,7 @@
         <v>44255</v>
       </c>
       <c r="D2" s="4">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="E2" s="8" t="str">
         <f>IF(A2="","",VLOOKUP(A2,HIDDEN!$E$2:$F$18,2,FALSE))</f>
@@ -4621,7 +4621,7 @@
         <v>44255</v>
       </c>
       <c r="D3" s="4">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="E3" s="8" t="str">
         <f>IF(A3="","",VLOOKUP(A3,HIDDEN!$E$2:$F$18,2,FALSE))</f>
@@ -4642,7 +4642,7 @@
         <v>43889</v>
       </c>
       <c r="D4" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E4" s="8" t="str">
         <f>IF(A4="","",VLOOKUP(A4,HIDDEN!$E$2:$F$18,2,FALSE))</f>
@@ -4663,7 +4663,7 @@
         <v>44255</v>
       </c>
       <c r="D5" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E5" s="8" t="str">
         <f>IF(A5="","",VLOOKUP(A5,HIDDEN!$E$2:$F$18,2,FALSE))</f>
@@ -5348,8 +5348,9 @@
       <formula1>1</formula1>
       <formula2>73051</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D100" xr:uid="{A6CC5939-A78C-BB46-8ED1-906DE28976E4}">
-      <formula1>INDIRECT(SUBSTITUTE(A2, " ", "_"))</formula1>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Value Range" prompt="Choose value:_x000a_ - between 0 and 3 for 'Transmissibility' and 'Lethality'_x000a_ - between 0 and 100 for 'Breakthrough infection probability'" sqref="D2:D100" xr:uid="{D0B6CB05-2BF1-9942-BA87-A771BD4402D5}">
+      <formula1>0</formula1>
+      <formula2>100</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7296,10 +7297,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:N153"/>
+  <dimension ref="A1:M153"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="O30" sqref="O30"/>
+    <sheetView topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
@@ -7315,7 +7316,7 @@
     <col min="15" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>333</v>
       </c>
@@ -7331,17 +7332,9 @@
       <c r="I1" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="M1" s="2"/>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="1" t="b">
         <v>0</v>
       </c>
@@ -7357,17 +7350,8 @@
       <c r="I2" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="L2" s="1">
-        <v>0</v>
-      </c>
-      <c r="M2" s="1">
-        <v>0</v>
-      </c>
-      <c r="N2" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="1" t="b">
         <v>1</v>
       </c>
@@ -7383,17 +7367,8 @@
       <c r="I3" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="L3" s="1">
-        <v>1</v>
-      </c>
-      <c r="M3" s="1">
-        <v>1</v>
-      </c>
-      <c r="N3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
+    </row>
+    <row r="4" spans="1:13">
       <c r="C4" s="1" t="s">
         <v>339</v>
       </c>
@@ -7403,17 +7378,8 @@
       <c r="F4" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="L4" s="1">
-        <v>2</v>
-      </c>
-      <c r="M4" s="1">
-        <v>2</v>
-      </c>
-      <c r="N4" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
+    </row>
+    <row r="5" spans="1:13">
       <c r="C5" s="1" t="s">
         <v>341</v>
       </c>
@@ -7423,17 +7389,8 @@
       <c r="F5" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="L5" s="1">
-        <v>3</v>
-      </c>
-      <c r="M5" s="1">
-        <v>3</v>
-      </c>
-      <c r="N5" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
+    </row>
+    <row r="6" spans="1:13">
       <c r="C6" s="1" t="s">
         <v>342</v>
       </c>
@@ -7443,11 +7400,8 @@
       <c r="F6" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="N6" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
+    </row>
+    <row r="7" spans="1:13">
       <c r="C7" s="1" t="s">
         <v>344</v>
       </c>
@@ -7457,11 +7411,8 @@
       <c r="F7" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="N7" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
+    </row>
+    <row r="8" spans="1:13">
       <c r="C8" s="1" t="s">
         <v>345</v>
       </c>
@@ -7471,11 +7422,8 @@
       <c r="F8" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="N8" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14">
+    </row>
+    <row r="9" spans="1:13">
       <c r="C9" s="1" t="s">
         <v>346</v>
       </c>
@@ -7485,11 +7433,8 @@
       <c r="F9" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="N9" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
+    </row>
+    <row r="10" spans="1:13">
       <c r="C10" s="1" t="s">
         <v>347</v>
       </c>
@@ -7499,11 +7444,8 @@
       <c r="F10" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="N10" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14">
+    </row>
+    <row r="11" spans="1:13">
       <c r="C11" s="1" t="s">
         <v>349</v>
       </c>
@@ -7513,11 +7455,8 @@
       <c r="F11" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="N11" s="1">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14">
+    </row>
+    <row r="12" spans="1:13">
       <c r="C12" s="1" t="s">
         <v>350</v>
       </c>
@@ -7527,11 +7466,8 @@
       <c r="F12" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="N12" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14">
+    </row>
+    <row r="13" spans="1:13">
       <c r="C13" s="1" t="s">
         <v>351</v>
       </c>
@@ -7541,11 +7477,8 @@
       <c r="F13" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="N13" s="1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14">
+    </row>
+    <row r="14" spans="1:13">
       <c r="C14" s="1" t="s">
         <v>353</v>
       </c>
@@ -7555,11 +7488,8 @@
       <c r="F14" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="N14" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14">
+    </row>
+    <row r="15" spans="1:13">
       <c r="C15" s="1" t="s">
         <v>354</v>
       </c>
@@ -7569,11 +7499,8 @@
       <c r="F15" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="N15" s="1">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14">
+    </row>
+    <row r="16" spans="1:13">
       <c r="C16" s="1" t="s">
         <v>356</v>
       </c>
@@ -7583,11 +7510,8 @@
       <c r="F16" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="N16" s="1">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="3:14">
+    </row>
+    <row r="17" spans="3:6">
       <c r="C17" s="1" t="s">
         <v>358</v>
       </c>
@@ -7597,11 +7521,8 @@
       <c r="F17" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="N17" s="1">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="3:14">
+    </row>
+    <row r="18" spans="3:6">
       <c r="C18" s="1" t="s">
         <v>359</v>
       </c>
@@ -7611,728 +7532,473 @@
       <c r="F18" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="N18" s="1">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="3:14">
+    </row>
+    <row r="19" spans="3:6">
       <c r="C19" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="N19" s="1">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="3:14">
+    </row>
+    <row r="20" spans="3:6">
       <c r="C20" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="N20" s="1">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="3:14">
+    </row>
+    <row r="21" spans="3:6">
       <c r="C21" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="N21" s="1">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="3:14">
+    </row>
+    <row r="22" spans="3:6">
       <c r="C22" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="N22" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="3:14">
+    </row>
+    <row r="23" spans="3:6">
       <c r="C23" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="N23" s="1">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="3:14">
+    </row>
+    <row r="24" spans="3:6">
       <c r="C24" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="N24" s="1">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="3:14">
+    </row>
+    <row r="25" spans="3:6">
       <c r="C25" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="N25" s="1">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="3:14">
+    </row>
+    <row r="26" spans="3:6">
       <c r="C26" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="N26" s="1">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="3:14">
+    </row>
+    <row r="27" spans="3:6">
       <c r="C27" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="N27" s="1">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="3:14">
+    </row>
+    <row r="28" spans="3:6">
       <c r="C28" s="1" t="s">
         <v>369</v>
       </c>
-      <c r="N28" s="1">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="3:14">
+    </row>
+    <row r="29" spans="3:6">
       <c r="C29" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="N29" s="1">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="3:14">
+    </row>
+    <row r="30" spans="3:6">
       <c r="C30" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="N30" s="1">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="3:14">
+    </row>
+    <row r="31" spans="3:6">
       <c r="C31" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="N31" s="1">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="32" spans="3:14">
+    </row>
+    <row r="32" spans="3:6">
       <c r="C32" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="N32" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="3:14">
+    </row>
+    <row r="33" spans="3:3">
       <c r="C33" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="N33" s="1">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="3:14">
+    </row>
+    <row r="34" spans="3:3">
       <c r="C34" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="N34" s="1">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="3:14">
+    </row>
+    <row r="35" spans="3:3">
       <c r="C35" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="N35" s="1">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="3:14">
+    </row>
+    <row r="36" spans="3:3">
       <c r="C36" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="N36" s="1">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="37" spans="3:14">
+    </row>
+    <row r="37" spans="3:3">
       <c r="C37" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="N37" s="1">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="38" spans="3:14">
+    </row>
+    <row r="38" spans="3:3">
       <c r="C38" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="N38" s="1">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="3:14">
+    </row>
+    <row r="39" spans="3:3">
       <c r="C39" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="N39" s="1">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="40" spans="3:14">
+    </row>
+    <row r="40" spans="3:3">
       <c r="C40" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="N40" s="1">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="41" spans="3:14">
+    </row>
+    <row r="41" spans="3:3">
       <c r="C41" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="N41" s="1">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="42" spans="3:14">
+    </row>
+    <row r="42" spans="3:3">
       <c r="C42" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="N42" s="1">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="43" spans="3:14">
+    </row>
+    <row r="43" spans="3:3">
       <c r="C43" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="N43" s="1">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="44" spans="3:14">
+    </row>
+    <row r="44" spans="3:3">
       <c r="C44" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="N44" s="1">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="45" spans="3:14">
+    </row>
+    <row r="45" spans="3:3">
       <c r="C45" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="N45" s="1">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="46" spans="3:14">
+    </row>
+    <row r="46" spans="3:3">
       <c r="C46" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="N46" s="1">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="47" spans="3:14">
+    </row>
+    <row r="47" spans="3:3">
       <c r="C47" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="N47" s="1">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="48" spans="3:14">
+    </row>
+    <row r="48" spans="3:3">
       <c r="C48" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="N48" s="1">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="49" spans="3:14">
+    </row>
+    <row r="49" spans="3:3">
       <c r="C49" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="N49" s="1">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="50" spans="3:14">
+    </row>
+    <row r="50" spans="3:3">
       <c r="C50" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="N50" s="1">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="51" spans="3:14">
+    </row>
+    <row r="51" spans="3:3">
       <c r="C51" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="N51" s="1">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="52" spans="3:14">
+    </row>
+    <row r="52" spans="3:3">
       <c r="C52" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="N52" s="1">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="53" spans="3:14">
+    </row>
+    <row r="53" spans="3:3">
       <c r="C53" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="N53" s="1">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="54" spans="3:14">
+    </row>
+    <row r="54" spans="3:3">
       <c r="C54" s="1" t="s">
         <v>395</v>
       </c>
-      <c r="N54" s="1">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="55" spans="3:14">
+    </row>
+    <row r="55" spans="3:3">
       <c r="C55" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="N55" s="1">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="56" spans="3:14">
+    </row>
+    <row r="56" spans="3:3">
       <c r="C56" s="1" t="s">
         <v>397</v>
       </c>
-      <c r="N56" s="1">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="57" spans="3:14">
+    </row>
+    <row r="57" spans="3:3">
       <c r="C57" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="N57" s="1">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="58" spans="3:14">
+    </row>
+    <row r="58" spans="3:3">
       <c r="C58" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="N58" s="1">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="59" spans="3:14">
+    </row>
+    <row r="59" spans="3:3">
       <c r="C59" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="N59" s="1">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="60" spans="3:14">
+    </row>
+    <row r="60" spans="3:3">
       <c r="C60" s="1" t="s">
         <v>401</v>
       </c>
-      <c r="N60" s="1">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="61" spans="3:14">
+    </row>
+    <row r="61" spans="3:3">
       <c r="C61" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="N61" s="1">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="62" spans="3:14">
+    </row>
+    <row r="62" spans="3:3">
       <c r="C62" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="N62" s="1">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="63" spans="3:14">
+    </row>
+    <row r="63" spans="3:3">
       <c r="C63" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="N63" s="1">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="64" spans="3:14">
+    </row>
+    <row r="64" spans="3:3">
       <c r="C64" s="1" t="s">
         <v>405</v>
       </c>
-      <c r="N64" s="1">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="65" spans="3:14">
+    </row>
+    <row r="65" spans="3:3">
       <c r="C65" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="N65" s="1">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="66" spans="3:14">
+    </row>
+    <row r="66" spans="3:3">
       <c r="C66" s="1" t="s">
         <v>407</v>
       </c>
-      <c r="N66" s="1">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="67" spans="3:14">
+    </row>
+    <row r="67" spans="3:3">
       <c r="C67" s="1" t="s">
         <v>408</v>
       </c>
-      <c r="N67" s="1">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="68" spans="3:14">
+    </row>
+    <row r="68" spans="3:3">
       <c r="C68" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="N68" s="1">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="69" spans="3:14">
+    </row>
+    <row r="69" spans="3:3">
       <c r="C69" s="1" t="s">
         <v>410</v>
       </c>
-      <c r="N69" s="1">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="70" spans="3:14">
+    </row>
+    <row r="70" spans="3:3">
       <c r="C70" s="1" t="s">
         <v>411</v>
       </c>
-      <c r="N70" s="1">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="71" spans="3:14">
+    </row>
+    <row r="71" spans="3:3">
       <c r="C71" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="N71" s="1">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="72" spans="3:14">
+    </row>
+    <row r="72" spans="3:3">
       <c r="C72" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="N72" s="1">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="73" spans="3:14">
+    </row>
+    <row r="73" spans="3:3">
       <c r="C73" s="1" t="s">
         <v>414</v>
       </c>
-      <c r="N73" s="1">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="74" spans="3:14">
+    </row>
+    <row r="74" spans="3:3">
       <c r="C74" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="N74" s="1">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="75" spans="3:14">
+    </row>
+    <row r="75" spans="3:3">
       <c r="C75" s="1" t="s">
         <v>416</v>
       </c>
-      <c r="N75" s="1">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="76" spans="3:14">
+    </row>
+    <row r="76" spans="3:3">
       <c r="C76" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="N76" s="1">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="77" spans="3:14">
+    </row>
+    <row r="77" spans="3:3">
       <c r="C77" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="N77" s="1">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="78" spans="3:14">
+    </row>
+    <row r="78" spans="3:3">
       <c r="C78" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="N78" s="1">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="79" spans="3:14">
+    </row>
+    <row r="79" spans="3:3">
       <c r="C79" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="N79" s="1">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="80" spans="3:14">
+    </row>
+    <row r="80" spans="3:3">
       <c r="C80" s="1" t="s">
         <v>421</v>
       </c>
-      <c r="N80" s="1">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="81" spans="3:14">
+    </row>
+    <row r="81" spans="3:3">
       <c r="C81" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="N81" s="1">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="82" spans="3:14">
+    </row>
+    <row r="82" spans="3:3">
       <c r="C82" s="1" t="s">
         <v>423</v>
       </c>
-      <c r="N82" s="1">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="83" spans="3:14">
+    </row>
+    <row r="83" spans="3:3">
       <c r="C83" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="N83" s="1">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="84" spans="3:14">
+    </row>
+    <row r="84" spans="3:3">
       <c r="C84" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="N84" s="1">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="85" spans="3:14">
+    </row>
+    <row r="85" spans="3:3">
       <c r="C85" s="1" t="s">
         <v>426</v>
       </c>
-      <c r="N85" s="1">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="86" spans="3:14">
+    </row>
+    <row r="86" spans="3:3">
       <c r="C86" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="N86" s="1">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="87" spans="3:14">
+    </row>
+    <row r="87" spans="3:3">
       <c r="C87" s="1" t="s">
         <v>428</v>
       </c>
-      <c r="N87" s="1">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="88" spans="3:14">
+    </row>
+    <row r="88" spans="3:3">
       <c r="C88" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="N88" s="1">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="89" spans="3:14">
+    </row>
+    <row r="89" spans="3:3">
       <c r="C89" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="N89" s="1">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="90" spans="3:14">
+    </row>
+    <row r="90" spans="3:3">
       <c r="C90" s="1" t="s">
         <v>431</v>
       </c>
-      <c r="N90" s="1">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="91" spans="3:14">
+    </row>
+    <row r="91" spans="3:3">
       <c r="C91" s="1" t="s">
         <v>432</v>
       </c>
-      <c r="N91" s="1">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="92" spans="3:14">
+    </row>
+    <row r="92" spans="3:3">
       <c r="C92" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="N92" s="1">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="93" spans="3:14">
+    </row>
+    <row r="93" spans="3:3">
       <c r="C93" s="1" t="s">
         <v>434</v>
       </c>
-      <c r="N93" s="1">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="94" spans="3:14">
+    </row>
+    <row r="94" spans="3:3">
       <c r="C94" s="1" t="s">
         <v>435</v>
       </c>
-      <c r="N94" s="1">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="95" spans="3:14">
+    </row>
+    <row r="95" spans="3:3">
       <c r="C95" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="N95" s="1">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="96" spans="3:14">
+    </row>
+    <row r="96" spans="3:3">
       <c r="C96" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="N96" s="1">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="97" spans="3:14">
+    </row>
+    <row r="97" spans="3:3">
       <c r="C97" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="N97" s="1">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="98" spans="3:14">
+    </row>
+    <row r="98" spans="3:3">
       <c r="C98" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="N98" s="1">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="99" spans="3:14">
+    </row>
+    <row r="99" spans="3:3">
       <c r="C99" s="1" t="s">
         <v>440</v>
       </c>
-      <c r="N99" s="1">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="100" spans="3:14">
+    </row>
+    <row r="100" spans="3:3">
       <c r="C100" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="N100" s="1">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="101" spans="3:14">
+    </row>
+    <row r="101" spans="3:3">
       <c r="C101" s="1" t="s">
         <v>442</v>
       </c>
-      <c r="N101" s="1">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="102" spans="3:14">
+    </row>
+    <row r="102" spans="3:3">
       <c r="C102" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="N102" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="103" spans="3:14">
+    </row>
+    <row r="103" spans="3:3">
       <c r="C103" s="1" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="104" spans="3:14">
+    <row r="104" spans="3:3">
       <c r="C104" s="1" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="105" spans="3:14">
+    <row r="105" spans="3:3">
       <c r="C105" s="1" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="106" spans="3:14">
+    <row r="106" spans="3:3">
       <c r="C106" s="1" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="107" spans="3:14">
+    <row r="107" spans="3:3">
       <c r="C107" s="1" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="108" spans="3:14">
+    <row r="108" spans="3:3">
       <c r="C108" s="1" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="109" spans="3:14">
+    <row r="109" spans="3:3">
       <c r="C109" s="1" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="110" spans="3:14">
+    <row r="110" spans="3:3">
       <c r="C110" s="1" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="111" spans="3:14">
+    <row r="111" spans="3:3">
       <c r="C111" s="1" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="112" spans="3:14">
+    <row r="112" spans="3:3">
       <c r="C112" s="1" t="s">
         <v>453</v>
       </c>

</xml_diff>